<commit_message>
Generación archivo salida paso 2
</commit_message>
<xml_diff>
--- a/website/Formatos/FormatoTDC_P2.xlsx
+++ b/website/Formatos/FormatoTDC_P2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APP\SitiosFuentes\qntProcesos\website\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APP\Sitios Fuentes\qntProcesos\website\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>IdColocacion</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Copia de NumeroTarjeta</t>
-  </si>
-  <si>
     <t>QNT EMPRESARIAL</t>
   </si>
   <si>
@@ -80,7 +77,13 @@
     <t>PENDIENTE ACUSE POR ALTA MAS.</t>
   </si>
   <si>
-    <t>RONALD*RODRIGUEZ</t>
+    <t>CopiadeNumeroTarjeta</t>
+  </si>
+  <si>
+    <t>NOMBRE1*APELLIDO1</t>
+  </si>
+  <si>
+    <t>ID_BPM</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +520,7 @@
     <col min="11" max="11" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,10 +552,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>6863</v>
       </c>
@@ -560,13 +566,13 @@
         <v>4813960</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="4">
         <v>200000</v>
@@ -575,7 +581,7 @@
         <v>901187660</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2">
         <v>201823</v>
@@ -584,7 +590,7 @@
         <v>15</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>